<commit_message>
Deploying to gh-pages from  @ 243ebd8465526e8a3ad6bb95e893ee0672ae2f8e 🚀
</commit_message>
<xml_diff>
--- a/2021-01-09.xlsx
+++ b/2021-01-09.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91741AAC-01F2-41D6-8396-535F7E0472BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F494FB6-19A0-43A1-88D7-4E8E954F4890}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="9" r:id="rId1"/>
-    <sheet name="Impfungen_bis_einschl_07.01.21" sheetId="6" r:id="rId2"/>
+    <sheet name="Impfungen_bis_einschl_08.01.21" sheetId="6" r:id="rId2"/>
     <sheet name="Impfungen_proTag" sheetId="10" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Bundesländer001" localSheetId="1">Impfungen_bis_einschl_07.01.21!$C$1:$I$17</definedName>
+    <definedName name="Bundesländer001" localSheetId="1">Impfungen_bis_einschl_08.01.21!$C$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -174,13 +174,13 @@
     <t>Impfungen gesamt</t>
   </si>
   <si>
-    <t>Durchgeführte Impfungen bundesweit und nach Bundesland sowie nach STIKO-Indikation bis einschließlich zum 07.01.21 (Impfungen_bis_einschl_07.01.21)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 07.01.21 durchgeführt und bis zum 08.01.21, 8:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
-  </si>
-  <si>
-    <t>Datenstand: 08.01.2021, 11:00 Uhr</t>
+    <t>Datenstand: 09.01.2021, 11:00 Uhr</t>
+  </si>
+  <si>
+    <t>Durchgeführte Impfungen bundesweit und nach Bundesland sowie nach STIKO-Indikation bis einschließlich 08.01.21 (Impfungen_bis_einschl_08.01.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 08.01.21 durchgeführt und bis zum 09.01.21, 11:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
   </si>
 </sst>
 </file>
@@ -859,10 +859,10 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="181.42578125" style="21" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="21"/>
@@ -880,7 +880,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
@@ -892,7 +892,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,7 +900,7 @@
     </row>
     <row r="7" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -949,7 +949,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,25 +999,25 @@
         <v>1</v>
       </c>
       <c r="C2" s="12">
-        <v>49103</v>
+        <v>55320</v>
       </c>
       <c r="D2" s="6">
-        <v>6180</v>
+        <v>6213</v>
       </c>
       <c r="E2" s="22">
-        <v>4.423536678067463</v>
+        <v>4.983606888187933</v>
       </c>
       <c r="F2" s="5">
-        <v>25827</v>
+        <v>29263</v>
       </c>
       <c r="G2" s="6">
-        <v>14560</v>
+        <v>16514</v>
       </c>
       <c r="H2" s="6">
-        <v>2433</v>
+        <v>2561</v>
       </c>
       <c r="I2" s="13">
-        <v>8088</v>
+        <v>9100</v>
       </c>
       <c r="J2" s="21"/>
     </row>
@@ -1029,25 +1029,25 @@
         <v>0</v>
       </c>
       <c r="C3" s="15">
-        <v>88916</v>
+        <v>93966</v>
       </c>
       <c r="D3" s="16">
-        <v>4567</v>
+        <v>5050</v>
       </c>
       <c r="E3" s="23">
-        <v>6.7746881327983948</v>
+        <v>7.1594577476104861</v>
       </c>
       <c r="F3" s="18">
-        <v>20212</v>
+        <v>20665</v>
       </c>
       <c r="G3" s="16">
-        <v>44516</v>
+        <v>47801</v>
       </c>
       <c r="H3" s="16">
-        <v>1609</v>
+        <v>1676</v>
       </c>
       <c r="I3" s="17">
-        <v>30110</v>
+        <v>31568</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1058,25 +1058,25 @@
         <v>3</v>
       </c>
       <c r="C4" s="12">
-        <v>26406</v>
+        <v>28871</v>
       </c>
       <c r="D4" s="6">
-        <v>2247</v>
+        <v>2465</v>
       </c>
       <c r="E4" s="22">
-        <v>7.1960934091403956</v>
+        <v>7.8678487016319156</v>
       </c>
       <c r="F4" s="5">
-        <v>16673</v>
+        <v>18591</v>
       </c>
       <c r="G4" s="6">
-        <v>9109</v>
+        <v>9676</v>
       </c>
       <c r="H4" s="6">
         <v>105</v>
       </c>
       <c r="I4" s="13">
-        <v>16773</v>
+        <v>18171</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1087,25 +1087,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="15">
-        <v>11481</v>
+        <v>13895</v>
       </c>
       <c r="D5" s="16">
-        <v>3299</v>
+        <v>2414</v>
       </c>
       <c r="E5" s="23">
-        <v>4.5525325618493726</v>
+        <v>5.5097500171498153</v>
       </c>
       <c r="F5" s="18">
-        <v>1029</v>
+        <v>1608</v>
       </c>
       <c r="G5" s="16">
-        <v>10391</v>
+        <v>12192</v>
       </c>
       <c r="H5" s="16">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="I5" s="17">
-        <v>558</v>
+        <v>908</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1116,25 +1116,25 @@
         <v>4</v>
       </c>
       <c r="C6" s="12">
-        <v>4505</v>
+        <v>5291</v>
       </c>
       <c r="D6" s="6">
-        <v>621</v>
+        <v>720</v>
       </c>
       <c r="E6" s="22">
-        <v>6.6133100020258304</v>
+        <v>7.7671527681950439</v>
       </c>
       <c r="F6" s="5">
-        <v>1033</v>
+        <v>1054</v>
       </c>
       <c r="G6" s="6">
-        <v>1764</v>
+        <v>2103</v>
       </c>
       <c r="H6" s="6">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I6" s="13">
-        <v>1491</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1145,25 +1145,25 @@
         <v>5</v>
       </c>
       <c r="C7" s="15">
-        <v>8471</v>
+        <v>9888</v>
       </c>
       <c r="D7" s="16">
-        <v>1392</v>
+        <v>1417</v>
       </c>
       <c r="E7" s="23">
-        <v>4.5857281054625441</v>
+        <v>5.352813068919092</v>
       </c>
       <c r="F7" s="18">
-        <v>2788</v>
+        <v>3172</v>
       </c>
       <c r="G7" s="16">
-        <v>4313</v>
+        <v>5188</v>
       </c>
       <c r="H7" s="16">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="I7" s="17">
-        <v>2352</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1174,25 +1174,25 @@
         <v>15</v>
       </c>
       <c r="C8" s="12">
-        <v>46006</v>
+        <v>48653</v>
       </c>
       <c r="D8" s="6">
-        <v>1884</v>
+        <v>2647</v>
       </c>
       <c r="E8" s="22">
-        <v>7.3163827432220963</v>
+        <v>7.7373379473543595</v>
       </c>
       <c r="F8" s="5">
-        <v>12286</v>
+        <v>12574</v>
       </c>
       <c r="G8" s="6">
-        <v>27009</v>
+        <v>28861</v>
       </c>
       <c r="H8" s="6">
-        <v>2101</v>
+        <v>2320</v>
       </c>
       <c r="I8" s="13">
-        <v>17520</v>
+        <v>18148</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1203,25 +1203,25 @@
         <v>6</v>
       </c>
       <c r="C9" s="15">
-        <v>24060</v>
+        <v>25141</v>
       </c>
       <c r="D9" s="16">
-        <v>1792</v>
+        <v>779</v>
       </c>
       <c r="E9" s="23">
-        <v>14.961402566197677</v>
+        <v>15.633608558469486</v>
       </c>
       <c r="F9" s="18">
-        <v>1260</v>
+        <v>1473</v>
       </c>
       <c r="G9" s="16">
-        <v>12515</v>
+        <v>13122</v>
       </c>
       <c r="H9" s="16">
-        <v>137</v>
+        <v>194</v>
       </c>
       <c r="I9" s="17">
-        <v>11130</v>
+        <v>11541</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1232,25 +1232,25 @@
         <v>7</v>
       </c>
       <c r="C10" s="12">
-        <v>32170</v>
+        <v>41646</v>
       </c>
       <c r="D10" s="6">
-        <v>7975</v>
+        <v>7803</v>
       </c>
       <c r="E10" s="22">
-        <v>4.02446554797283</v>
+        <v>5.2099127202634907</v>
       </c>
       <c r="F10" s="5">
-        <v>7075</v>
+        <v>9369</v>
       </c>
       <c r="G10" s="6">
-        <v>15989</v>
+        <v>20483</v>
       </c>
       <c r="H10" s="6">
-        <v>6226</v>
+        <v>7978</v>
       </c>
       <c r="I10" s="13">
-        <v>18332</v>
+        <v>22615</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1261,25 +1261,25 @@
         <v>8</v>
       </c>
       <c r="C11" s="15">
-        <v>90802</v>
+        <v>98950</v>
       </c>
       <c r="D11" s="16">
-        <v>5986</v>
+        <v>6574</v>
       </c>
       <c r="E11" s="23">
-        <v>5.0593905318266268</v>
+        <v>5.5133883958970582</v>
       </c>
       <c r="F11" s="18">
         <v>0</v>
       </c>
       <c r="G11" s="16">
-        <v>39465</v>
+        <v>43671</v>
       </c>
       <c r="H11" s="16">
         <v>0</v>
       </c>
       <c r="I11" s="17">
-        <v>51345</v>
+        <v>55287</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1290,25 +1290,25 @@
         <v>12</v>
       </c>
       <c r="C12" s="12">
-        <v>20792</v>
+        <v>25482</v>
       </c>
       <c r="D12" s="6">
-        <v>4991</v>
+        <v>4376</v>
       </c>
       <c r="E12" s="22">
-        <v>5.0787720178030602</v>
+        <v>6.2243780568323182</v>
       </c>
       <c r="F12" s="5">
-        <v>2154</v>
+        <v>3777</v>
       </c>
       <c r="G12" s="6">
-        <v>11833</v>
+        <v>14104</v>
       </c>
       <c r="H12" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I12" s="13">
-        <v>6805</v>
+        <v>7597</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1319,25 +1319,25 @@
         <v>13</v>
       </c>
       <c r="C13" s="15">
-        <v>7358</v>
+        <v>8232</v>
       </c>
       <c r="D13" s="16">
-        <v>837</v>
+        <v>874</v>
       </c>
       <c r="E13" s="23">
-        <v>7.4557674789514907</v>
+        <v>8.3413805227954168</v>
       </c>
       <c r="F13" s="18">
-        <v>5596</v>
+        <v>6236</v>
       </c>
       <c r="G13" s="16">
-        <v>966</v>
+        <v>1104</v>
       </c>
       <c r="H13" s="16">
         <v>0</v>
       </c>
       <c r="I13" s="17">
-        <v>2663</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,25 +1348,25 @@
         <v>9</v>
       </c>
       <c r="C14" s="12">
-        <v>15593</v>
+        <v>17991</v>
       </c>
       <c r="D14" s="6">
-        <v>2587</v>
+        <v>2398</v>
       </c>
       <c r="E14" s="22">
-        <v>3.8293494722825874</v>
+        <v>4.4182534698798195</v>
       </c>
       <c r="F14" s="5">
-        <v>985</v>
+        <v>1024</v>
       </c>
       <c r="G14" s="6">
-        <v>13343</v>
+        <v>15283</v>
       </c>
       <c r="H14" s="6">
         <v>1</v>
       </c>
       <c r="I14" s="13">
-        <v>2249</v>
+        <v>2707</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1377,25 +1377,25 @@
         <v>10</v>
       </c>
       <c r="C15" s="15">
-        <v>19399</v>
+        <v>20799</v>
       </c>
       <c r="D15" s="16">
-        <v>1775</v>
+        <v>1400</v>
       </c>
       <c r="E15" s="23">
-        <v>8.8386910408414145</v>
+        <v>9.4765676044363421</v>
       </c>
       <c r="F15" s="18">
-        <v>6008</v>
+        <v>6427</v>
       </c>
       <c r="G15" s="16">
-        <v>9554</v>
+        <v>10228</v>
       </c>
       <c r="H15" s="16">
-        <v>783</v>
+        <v>987</v>
       </c>
       <c r="I15" s="17">
-        <v>9500</v>
+        <v>10214</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1406,25 +1406,25 @@
         <v>11</v>
       </c>
       <c r="C16" s="12">
-        <v>23903</v>
+        <v>28241</v>
       </c>
       <c r="D16" s="6">
-        <v>3831</v>
+        <v>3936</v>
       </c>
       <c r="E16" s="22">
-        <v>8.2317040622665747</v>
+        <v>9.7256224918407881</v>
       </c>
       <c r="F16" s="5">
-        <v>5606</v>
+        <v>6486</v>
       </c>
       <c r="G16" s="6">
-        <v>10747</v>
+        <v>12623</v>
       </c>
       <c r="H16" s="6">
-        <v>3655</v>
+        <v>3947</v>
       </c>
       <c r="I16" s="13">
-        <v>9099</v>
+        <v>10551</v>
       </c>
       <c r="J16" s="21"/>
     </row>
@@ -1436,25 +1436,25 @@
         <v>14</v>
       </c>
       <c r="C17" s="15">
-        <v>7994</v>
+        <v>10512</v>
       </c>
       <c r="D17" s="16">
-        <v>974</v>
+        <v>1000</v>
       </c>
       <c r="E17" s="23">
-        <v>3.7471090449043727</v>
+        <v>4.9273968326288173</v>
       </c>
       <c r="F17" s="16">
-        <v>782</v>
+        <v>903</v>
       </c>
       <c r="G17" s="16">
-        <v>6399</v>
+        <v>8583</v>
       </c>
       <c r="H17" s="16">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I17" s="17">
-        <v>731</v>
+        <v>924</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1464,31 +1464,31 @@
       </c>
       <c r="C18" s="14">
         <f>SUM(C2:C17)</f>
-        <v>476959</v>
+        <v>532878</v>
       </c>
       <c r="D18" s="14">
         <f>SUM(D2:D17)</f>
-        <v>50938</v>
+        <v>50066</v>
       </c>
       <c r="E18" s="24">
         <f>C18/83166711*1000</f>
-        <v>5.7349748987909361</v>
+        <v>6.4073472858629694</v>
       </c>
       <c r="F18" s="7">
         <f>SUM(F2:F17)</f>
-        <v>109314</v>
+        <v>122622</v>
       </c>
       <c r="G18" s="8">
         <f>SUM(G2:G17)</f>
-        <v>232473</v>
+        <v>261536</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" ref="H18:I18" si="0">SUM(H2:H17)</f>
-        <v>17267</v>
+        <v>20043</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="0"/>
-        <v>188746</v>
+        <v>206772</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926B42D2-7956-44E7-BD5B-5AF896796AC0}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1541,7 +1543,7 @@
         <v>44192</v>
       </c>
       <c r="B2" s="36">
-        <v>23622</v>
+        <v>23621</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1549,7 +1551,7 @@
         <v>44193</v>
       </c>
       <c r="B3" s="36">
-        <v>18960</v>
+        <v>19060</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1557,7 +1559,7 @@
         <v>44194</v>
       </c>
       <c r="B4" s="36">
-        <v>42152</v>
+        <v>42254</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1565,7 +1567,7 @@
         <v>44195</v>
       </c>
       <c r="B5" s="36">
-        <v>56519</v>
+        <v>56562</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1573,7 +1575,7 @@
         <v>44196</v>
       </c>
       <c r="B6" s="36">
-        <v>37235</v>
+        <v>37533</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1581,7 +1583,7 @@
         <v>44197</v>
       </c>
       <c r="B7" s="36">
-        <v>30212</v>
+        <v>30213</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1589,7 +1591,7 @@
         <v>44198</v>
       </c>
       <c r="B8" s="36">
-        <v>44400</v>
+        <v>44458</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1597,7 +1599,7 @@
         <v>44199</v>
       </c>
       <c r="B9" s="36">
-        <v>24237</v>
+        <v>24236</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1605,7 +1607,7 @@
         <v>44200</v>
       </c>
       <c r="B10" s="36">
-        <v>47441</v>
+        <v>47497</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1613,7 +1615,7 @@
         <v>44201</v>
       </c>
       <c r="B11" s="36">
-        <v>48252</v>
+        <v>49176</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1621,7 +1623,7 @@
         <v>44202</v>
       </c>
       <c r="B12" s="36">
-        <v>52991</v>
+        <v>53665</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1630,7 +1632,15 @@
         <v>44203</v>
       </c>
       <c r="B13" s="36">
-        <v>50938</v>
+        <v>54537</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <v>44204</v>
+      </c>
+      <c r="B14" s="36">
+        <v>50066</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1639,7 +1649,7 @@
       </c>
       <c r="B21" s="35">
         <f>SUM(B2:B17)</f>
-        <v>476959</v>
+        <v>532878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>